<commit_message>
Fixed data transfer issue in admin panel
</commit_message>
<xml_diff>
--- a/packages/Webkul/Admin/tests/e2e-pw/data/data-transfer/products.xlsx
+++ b/packages/Webkul/Admin/tests/e2e-pw/data/data-transfer/products.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="115">
   <si>
     <t xml:space="preserve">sku</t>
   </si>
@@ -134,6 +134,9 @@
   </si>
   <si>
     <t xml:space="preserve">associated_skus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rma_rule_id</t>
   </si>
   <si>
     <t xml:space="preserve">SP-001</t>
@@ -377,6 +380,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -436,9 +440,13 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -462,13 +470,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AL12"/>
+  <dimension ref="A1:AM12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O3" activeCellId="0" sqref="O3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G22" activeCellId="0" sqref="G22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.44"/>
@@ -476,27 +484,27 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="19.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="19.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="49.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="0" width="0.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="6.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="16.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="4.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="8.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="14.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="14.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="6.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="5.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="5.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="6.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="6.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="17.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="5.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="5.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="5.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="12.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="16.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="16.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="14.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="62.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="46.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="9.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="9.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="18.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="15.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="13.36"/>
@@ -506,7 +514,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="0" width="14.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="0" width="109.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="0" width="255.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="0" width="26.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="0" width="26.85"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -624,34 +632,37 @@
       <c r="AL1" s="0" t="s">
         <v>37</v>
       </c>
+      <c r="AM1" s="1" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="K2" s="0" t="n">
         <v>1</v>
@@ -669,63 +680,66 @@
         <v>14</v>
       </c>
       <c r="Z2" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AA2" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="AB2" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="AC2" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="AD2" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="AE2" s="0" t="n">
         <v>1</v>
       </c>
       <c r="AF2" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="AG2" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="AH2" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="AI2" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
+      </c>
+      <c r="AM2" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="K3" s="0" t="n">
         <v>1</v>
@@ -743,60 +757,63 @@
         <v>17</v>
       </c>
       <c r="AA3" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AB3" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="AC3" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="AD3" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="AE3" s="0" t="n">
         <v>1</v>
       </c>
       <c r="AF3" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="AG3" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AH3" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AI3" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
+      </c>
+      <c r="AM3" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K4" s="0" t="n">
         <v>1</v>
@@ -816,67 +833,70 @@
       <c r="W4" s="0" t="n">
         <v>17</v>
       </c>
-      <c r="X4" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="Y4" s="1" t="s">
+      <c r="X4" s="2" t="s">
         <v>67</v>
       </c>
+      <c r="Y4" s="2" t="s">
+        <v>68</v>
+      </c>
       <c r="AA4" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="AB4" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="AC4" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="AD4" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="AE4" s="0" t="n">
         <v>1</v>
       </c>
       <c r="AF4" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="AG4" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="AH4" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="AI4" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
+      </c>
+      <c r="AM4" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="K5" s="0" t="n">
         <v>1</v>
@@ -894,60 +914,63 @@
         <v>21</v>
       </c>
       <c r="AA5" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="AB5" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="AC5" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="AD5" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="AE5" s="0" t="n">
         <v>1</v>
       </c>
       <c r="AF5" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="AG5" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="AH5" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="AI5" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
+      </c>
+      <c r="AM5" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="J6" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="K6" s="0" t="n">
         <v>1</v>
@@ -959,48 +982,51 @@
         <v>0</v>
       </c>
       <c r="AA6" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="AB6" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="AC6" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="AD6" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="AL6" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
+      </c>
+      <c r="AM6" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="J7" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="K7" s="0" t="n">
         <v>1</v>
@@ -1012,48 +1038,51 @@
         <v>0</v>
       </c>
       <c r="AA7" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="AB7" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="AC7" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="AD7" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="AK7" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
+      </c>
+      <c r="AM7" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="J8" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="K8" s="0" t="n">
         <v>1</v>
@@ -1065,51 +1094,54 @@
         <v>0</v>
       </c>
       <c r="AA8" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="AB8" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="AC8" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="AD8" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="AJ8" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
+      </c>
+      <c r="AM8" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="J9" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="K9" s="0" t="n">
         <v>1</v>
@@ -1127,54 +1159,57 @@
         <v>14</v>
       </c>
       <c r="AA9" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="AB9" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="AC9" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="AD9" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="AE9" s="0" t="n">
         <v>1</v>
       </c>
       <c r="AF9" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
+      </c>
+      <c r="AM9" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="J10" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="K10" s="0" t="n">
         <v>1</v>
@@ -1192,54 +1227,57 @@
         <v>17</v>
       </c>
       <c r="AA10" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="AB10" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="AC10" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="AD10" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="AE10" s="0" t="n">
         <v>1</v>
       </c>
       <c r="AF10" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
+      </c>
+      <c r="AM10" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="J11" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="K11" s="0" t="n">
         <v>1</v>
@@ -1259,61 +1297,64 @@
       <c r="W11" s="0" t="n">
         <v>17</v>
       </c>
-      <c r="X11" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="Y11" s="1" t="s">
+      <c r="X11" s="2" t="s">
         <v>67</v>
       </c>
+      <c r="Y11" s="2" t="s">
+        <v>68</v>
+      </c>
       <c r="AA11" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="AB11" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="AC11" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="AD11" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="AE11" s="0" t="n">
         <v>1</v>
       </c>
       <c r="AF11" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
+      </c>
+      <c r="AM11" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="J12" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="K12" s="0" t="n">
         <v>1</v>
@@ -1333,35 +1374,38 @@
       <c r="W12" s="0" t="n">
         <v>17</v>
       </c>
-      <c r="X12" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="Y12" s="1" t="s">
+      <c r="X12" s="2" t="s">
         <v>67</v>
       </c>
+      <c r="Y12" s="2" t="s">
+        <v>68</v>
+      </c>
       <c r="AA12" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AB12" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="AC12" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="AD12" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="AE12" s="0" t="n">
         <v>1</v>
       </c>
       <c r="AF12" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
+      </c>
+      <c r="AM12" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>